<commit_message>
update AT0029 download template
</commit_message>
<xml_diff>
--- a/data/Example/Setting.xlsx
+++ b/data/Example/Setting.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\DRJ Automation\data\Example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaProjects\service-selenium-automation\data\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3805C9-A2F8-4A5C-9D69-CBEFFC519C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="2580" windowWidth="21495" windowHeight="11220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="2580" windowWidth="21495" windowHeight="11220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -105,8 +104,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -482,14 +481,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" customWidth="1"/>
@@ -501,7 +500,7 @@
     <col min="1020" max="1022" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14.25">
+    <row r="1" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +547,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="14.25">
+    <row r="2" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -562,7 +561,7 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <v>202410</v>
+        <v>202504</v>
       </c>
       <c r="F2" t="s">
         <v>22</v>
@@ -580,10 +579,10 @@
         <v>18</v>
       </c>
       <c r="K2">
-        <v>20241004</v>
+        <v>20250304</v>
       </c>
       <c r="L2">
-        <v>20241103</v>
+        <v>20250403</v>
       </c>
       <c r="N2" t="b">
         <v>1</v>
@@ -592,7 +591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14.25">
+    <row r="3" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -612,52 +611,52 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="14.25">
+    <row r="4" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="14.25">
+    <row r="5" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="14.25">
+    <row r="6" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="14.25">
+    <row r="7" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="14.25">
+    <row r="8" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="14.25">
+    <row r="9" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="14.25">
+    <row r="10" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="14.25">
+    <row r="11" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="14.25">
+    <row r="12" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:15" ht="14.25">
+    <row r="13" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>

</xml_diff>